<commit_message>
2016-06-09掠夺(进攻-秦字-九华-紫阳总舵) YY_List & Valid_List Update
</commit_message>
<xml_diff>
--- a/compare.xlsx
+++ b/compare.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="154">
   <si>
     <t>池小晚</t>
   </si>
@@ -42,27 +42,18 @@
     <t>阿木木</t>
   </si>
   <si>
-    <t>与尔同销萬古愁</t>
-  </si>
-  <si>
     <t>浪迹小秦</t>
   </si>
   <si>
     <t>一直梨花压海棠</t>
   </si>
   <si>
-    <t>零拾</t>
-  </si>
-  <si>
     <t>凌渃尘</t>
   </si>
   <si>
     <t>素蝶</t>
   </si>
   <si>
-    <t>只想做个好人</t>
-  </si>
-  <si>
     <t>折扇浪漫</t>
   </si>
   <si>
@@ -75,21 +66,12 @@
     <t>小阿淮呀</t>
   </si>
   <si>
-    <t>明年今日奕十年</t>
-  </si>
-  <si>
     <t>梦觞丶</t>
   </si>
   <si>
-    <t>青丝枫凌</t>
-  </si>
-  <si>
     <t>墨河</t>
   </si>
   <si>
-    <t>荡荡</t>
-  </si>
-  <si>
     <t>其实想玩刀客</t>
   </si>
   <si>
@@ -117,9 +99,6 @@
     <t>那年今若、</t>
   </si>
   <si>
-    <t>小阿鏡</t>
-  </si>
-  <si>
     <t>伊贰叁</t>
   </si>
   <si>
@@ -141,9 +120,6 @@
     <t>神威再见</t>
   </si>
   <si>
-    <t>Ander</t>
-  </si>
-  <si>
     <t>超人不会飞〃</t>
   </si>
   <si>
@@ -177,18 +153,9 @@
     <t>等风与你</t>
   </si>
   <si>
-    <t>风语风＊</t>
-  </si>
-  <si>
     <t>在下唐言</t>
   </si>
   <si>
-    <t>与尔同</t>
-  </si>
-  <si>
-    <t>小狼</t>
-  </si>
-  <si>
     <t>浪迹</t>
   </si>
   <si>
@@ -204,24 +171,15 @@
     <t>山高</t>
   </si>
   <si>
-    <t>洪时</t>
-  </si>
-  <si>
     <t>潇洒</t>
   </si>
   <si>
-    <t>天蓝色</t>
-  </si>
-  <si>
     <t>晓月梦</t>
   </si>
   <si>
     <t>陌路莫回</t>
   </si>
   <si>
-    <t>南宫</t>
-  </si>
-  <si>
     <t>凯贼</t>
   </si>
   <si>
@@ -246,24 +204,12 @@
     <t>白芹</t>
   </si>
   <si>
-    <t>胡大力</t>
-  </si>
-  <si>
     <t>紫舞流年</t>
   </si>
   <si>
     <t>墨韵轩华</t>
   </si>
   <si>
-    <t>苏千澪</t>
-  </si>
-  <si>
-    <t>娇软の小屁股</t>
-  </si>
-  <si>
-    <t>青羽墨染云</t>
-  </si>
-  <si>
     <t>天真无邪大胡子</t>
   </si>
   <si>
@@ -273,114 +219,42 @@
     <t>淡若清风過丶</t>
   </si>
   <si>
-    <t>似有若无</t>
-  </si>
-  <si>
-    <t>破穿</t>
-  </si>
-  <si>
-    <t>＊团灭专用奶</t>
-  </si>
-  <si>
-    <t>眉间一点白</t>
-  </si>
-  <si>
-    <t>机智勇敢的小炮</t>
-  </si>
-  <si>
-    <t>东瀛浪人展梦魂</t>
-  </si>
-  <si>
     <t>一个有内涵的人</t>
   </si>
   <si>
-    <t>梦离间丶</t>
-  </si>
-  <si>
-    <t>岚风夜雨</t>
-  </si>
-  <si>
     <t>倾舞情儿</t>
   </si>
   <si>
     <t>丐帮萌主</t>
   </si>
   <si>
-    <t>FateLibra</t>
-  </si>
-  <si>
-    <t>Northenhumilia</t>
-  </si>
-  <si>
     <t>彼眸</t>
   </si>
   <si>
-    <t>慕容靉</t>
-  </si>
-  <si>
     <t>艾莉亞史塔克</t>
   </si>
   <si>
-    <t>方得始終</t>
-  </si>
-  <si>
-    <t>凶光外露的熊</t>
-  </si>
-  <si>
-    <t>丨龙哥丿</t>
-  </si>
-  <si>
-    <t>剑泣天涯</t>
-  </si>
-  <si>
-    <t>歌风路丶三狗蛋</t>
-  </si>
-  <si>
     <t>凌</t>
   </si>
   <si>
-    <t>小屁</t>
-  </si>
-  <si>
     <t>折扇</t>
   </si>
   <si>
-    <t>明年今</t>
-  </si>
-  <si>
     <t>梦觞</t>
   </si>
   <si>
     <t>内涵</t>
   </si>
   <si>
-    <t>太极至</t>
-  </si>
-  <si>
-    <t>小炮</t>
-  </si>
-  <si>
     <t>淺</t>
   </si>
   <si>
-    <t>湳枝</t>
-  </si>
-  <si>
     <t>三狗蛋</t>
   </si>
   <si>
-    <t>萧四</t>
-  </si>
-  <si>
     <t>淡若</t>
   </si>
   <si>
-    <t>艾莉亞史</t>
-  </si>
-  <si>
-    <t>一抹煙雨</t>
-  </si>
-  <si>
     <t>忍野咩咩</t>
   </si>
   <si>
@@ -405,25 +279,211 @@
     <t>轻素剪云</t>
   </si>
   <si>
-    <t>风语风</t>
-  </si>
-  <si>
-    <t>吕小</t>
-  </si>
-  <si>
-    <t>百里</t>
-  </si>
-  <si>
-    <t>青丝</t>
-  </si>
-  <si>
-    <t>何月</t>
-  </si>
-  <si>
     <t>伊</t>
   </si>
   <si>
-    <t>甄</t>
+    <t>紫雨幽雲</t>
+  </si>
+  <si>
+    <t>古巷烟雨断桥殇</t>
+  </si>
+  <si>
+    <t>独孤沐白</t>
+  </si>
+  <si>
+    <t>百里轩翊</t>
+  </si>
+  <si>
+    <t>唐糖～</t>
+  </si>
+  <si>
+    <t>框框</t>
+  </si>
+  <si>
+    <t>天韵ゝ</t>
+  </si>
+  <si>
+    <t>丶初馨</t>
+  </si>
+  <si>
+    <t>只会躺不输出丶</t>
+  </si>
+  <si>
+    <t>异逍遥</t>
+  </si>
+  <si>
+    <t>椛灯</t>
+  </si>
+  <si>
+    <t>丿几度度丶</t>
+  </si>
+  <si>
+    <t>守护锋</t>
+  </si>
+  <si>
+    <t>鱼小小</t>
+  </si>
+  <si>
+    <t>薄霭</t>
+  </si>
+  <si>
+    <t>东风路三狗蛋</t>
+  </si>
+  <si>
+    <t>永恒只为等待</t>
+  </si>
+  <si>
+    <t>巡山的人</t>
+  </si>
+  <si>
+    <t>萌萌哒的草莓酱</t>
+  </si>
+  <si>
+    <t>盖世呆头洋</t>
+  </si>
+  <si>
+    <t>凰荼歌</t>
+  </si>
+  <si>
+    <t>い楓ゞ妖い</t>
+  </si>
+  <si>
+    <t>微微醉的葫芦酱</t>
+  </si>
+  <si>
+    <t>骑驴不喝酒</t>
+  </si>
+  <si>
+    <t>浅浅笑的梅子酱</t>
+  </si>
+  <si>
+    <t>唐舞桐灬</t>
+  </si>
+  <si>
+    <t>友善的小内衣</t>
+  </si>
+  <si>
+    <t>一将羽霄一</t>
+  </si>
+  <si>
+    <t>乌莲娜</t>
+  </si>
+  <si>
+    <t>诸天花雨</t>
+  </si>
+  <si>
+    <t>一息衍一</t>
+  </si>
+  <si>
+    <t>儒丶张良</t>
+  </si>
+  <si>
+    <t>男人应有的自豪</t>
+  </si>
+  <si>
+    <t>等我出轻语</t>
+  </si>
+  <si>
+    <t>芝麻花生馅儿饺</t>
+  </si>
+  <si>
+    <t>浩浩丶浩</t>
+  </si>
+  <si>
+    <t>慕容飞羽</t>
+  </si>
+  <si>
+    <t>淺笙</t>
+  </si>
+  <si>
+    <t>蝶舞旧梦</t>
+  </si>
+  <si>
+    <t>纯洁友善的暮夏</t>
+  </si>
+  <si>
+    <t>Yennefer</t>
+  </si>
+  <si>
+    <t>绫月薇</t>
+  </si>
+  <si>
+    <t>劍問兲涯覓紅颜</t>
+  </si>
+  <si>
+    <t>古巷烟雨</t>
+  </si>
+  <si>
+    <t>只会躺不输出</t>
+  </si>
+  <si>
+    <t>妖</t>
+  </si>
+  <si>
+    <t>几度</t>
+  </si>
+  <si>
+    <t>初馨</t>
+  </si>
+  <si>
+    <t>唐糖</t>
+  </si>
+  <si>
+    <t>天韵</t>
+  </si>
+  <si>
+    <t>永恒</t>
+  </si>
+  <si>
+    <t>一抹煙雨落</t>
+  </si>
+  <si>
+    <t>男人应有</t>
+  </si>
+  <si>
+    <t>盖世呆头</t>
+  </si>
+  <si>
+    <t>张良</t>
+  </si>
+  <si>
+    <t>奶小牛</t>
+  </si>
+  <si>
+    <t>梅子</t>
+  </si>
+  <si>
+    <t>水影</t>
+  </si>
+  <si>
+    <t>浩浩</t>
+  </si>
+  <si>
+    <t>友善的暮夏</t>
+  </si>
+  <si>
+    <t>荡荡</t>
+  </si>
+  <si>
+    <t>葫芦</t>
+  </si>
+  <si>
+    <t>那年今</t>
+  </si>
+  <si>
+    <t>鹰老七</t>
+  </si>
+  <si>
+    <t>炮</t>
+  </si>
+  <si>
+    <t>在下唐</t>
+  </si>
+  <si>
+    <t>萧四无</t>
+  </si>
+  <si>
+    <t>寻</t>
   </si>
 </sst>
 </file>
@@ -742,11 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C584"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,1025 +817,1157 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C1" t="str">
         <f>VLOOKUP("*"&amp;A1&amp;"*",B:B,1,0)</f>
-        <v>与尔同销萬古愁</v>
+        <v>凌渃尘</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C65" si="0">VLOOKUP("*"&amp;A2&amp;"*",B:B,1,0)</f>
-        <v>青丝枫凌</v>
+        <v>南宫絮语</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>南宫絮语</v>
+        <v>古巷烟雨断桥殇</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>只想做个好人</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>只会躺不输出丶</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>墨河</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>墨河</v>
+        <v>女神菲奥娜</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>女神菲奥娜</v>
+        <v>异逍遥</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>娇软の小屁股</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>折扇浪漫</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>89</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>梦觞丶</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>折扇浪漫</v>
+        <v>浪迹小秦</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>明年今日奕十年</v>
+        <v>一直梨花压海棠</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>梦觞丶</v>
+        <v>独孤沐白</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>浪迹小秦</v>
+        <v>百里轩翊</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>一直梨花压海棠</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>素蝶</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>51</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>小阿淮呀</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>破穿</v>
+        <v>い楓ゞ妖い</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>素蝶</v>
+        <v>倾舞情儿</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>小阿淮呀</v>
+        <v>一个有内涵的人</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>132</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>零拾</v>
+        <v>丿几度度丶</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>青丝枫凌</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>丶初馨</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>62</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>唐糖～</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>倾舞情儿</v>
+        <v>墨韵轩华</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>一个有内涵的人</v>
+        <v>天韵ゝ</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>墨韵轩华</v>
+        <v>19</v>
+      </c>
+      <c r="C24" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>太极至尊</v>
+        <v>怒怒怒怒火</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>机智勇敢的小炮</v>
+        <v>慕容飞羽</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>怒怒怒怒火</v>
+        <v>椛灯</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>永恒只为等待</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="1" t="str">
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>池小晚</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>94</v>
+      </c>
+      <c r="C30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>池小猫</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="C31" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>爱哭鼻の阿木木</v>
+        <v>淺笙</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>歌风路丶三狗蛋</v>
+        <v>诸天花雨</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>伊贰叁</v>
+        <v>爱哭鼻の阿木木</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>137</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>其实想玩刀客</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>一抹煙雨落繁華</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>96</v>
+      </c>
+      <c r="C35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>乌莲娜</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="C36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>在下唐银</v>
+        <v>冷清语</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>空虚公子萧四无</v>
+        <v>在下唐言</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C38" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>山高丶木易</v>
+        <v>墨萧炎</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>开封拍卖行</v>
+        <v>丶忍野咩咩</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C40" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>彼眸</v>
+        <v>晓月梦澈</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>慕容靉</v>
+        <v>凯贼阔里</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C42" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>山高丶木易</v>
+        <v>榕月</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="C43" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>水影悠兰</v>
+        <v>沐浠尘</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>138</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C44" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>洪时雪</v>
+        <v>男人应有的自豪</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>淡若清风過丶</v>
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="C46" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>潇洒仗剑天下</v>
+        <v>盖世呆头洋</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C47" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>紫舞流年</v>
+        <v>神威再见</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="C48" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>艾莉亞史塔克</v>
+        <v>等风与你</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="C49" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>池小猫</v>
+        <v>再见是否红着脸</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C50" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Ander</v>
+        <v>天真无邪大胡子</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C51" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>一抹煙雨落繁華</v>
+        <v>花谢人凋零。</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>冷清语</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>超人不会飞〃</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>68</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>轻素剪云端</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="C54" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>丶天蓝色</v>
+        <v>陌路莫回</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="C55" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>丶忍野咩咩</v>
+        <v>鱼小小</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C56" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>晓月梦澈</v>
+        <v>鱼香</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="C57" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>凯贼阔里</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>东风路三狗蛋</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C58" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>108</v>
+      </c>
+      <c r="C58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>伊贰叁</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>49</v>
+        <v>140</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="C59" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>沐浠尘</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>儒丶张良</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>47</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>9</v>
+      </c>
+      <c r="C60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>其实想玩刀客</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="C61" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>白芹</v>
+        <v>在下唐银</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>152</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>神威再见</v>
+        <v>空虚公子萧四无</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>等风与你</v>
+        <v>奶小牛丶</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>48</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C64" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>再见是否红着脸</v>
+        <v>山高丶木易</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="C65" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>胡大力</v>
+        <v>开封拍卖行</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>68</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="C66" s="1" t="str">
-        <f t="shared" ref="C66:C75" si="1">VLOOKUP("*"&amp;A66&amp;"*",B:B,1,0)</f>
-        <v>天真无邪大胡子</v>
+        <f t="shared" ref="C66:C86" si="1">VLOOKUP("*"&amp;A66&amp;"*",B:B,1,0)</f>
+        <v>彼眸</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C67" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>花谢人凋零。</v>
+        <v>山高丶木易</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C68" s="1" t="str">
+        <v>113</v>
+      </c>
+      <c r="C68" s="1" t="e">
         <f t="shared" si="1"/>
-        <v>超人不会飞〃</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="C69" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>轻素剪云端</v>
+        <v>框框</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>142</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="C70" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>陌路莫回</v>
+        <v>浅浅笑的梅子酱</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C71" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>风语风＊</v>
+        <v>水影悠兰</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C72" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>鱼香</v>
+        <v>洪时雪</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>144</v>
+      </c>
       <c r="B73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C73" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>浩浩丶浩</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C74" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>淡若清风過丶</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C75" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>潇洒仗剑天下</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>等我出轻语</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>60</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>紫舞流年</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>紫雨幽雲</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>纯洁友善的暮夏</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>69</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>艾莉亞史塔克</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>146</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C81" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>147</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>微微醉的葫芦酱</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>100</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>薄霭</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C84" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>那年今若、</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="1"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" s="1"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="1" t="s">
+      <c r="B85" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C85" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>那年红颜</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>149</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C86" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>追风少年鹰老七</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C96" s="1"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C97" s="1"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="C98" s="1"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C99" s="1"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C100" s="1"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C102" s="1"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C103" s="1"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C104" s="1"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C105" s="1"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C106" s="1"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C112" s="1"/>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
@@ -3196,71 +3387,7 @@
       <c r="C584" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C572">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="Ander"/>
-        <filter val="一个有内涵的人"/>
-        <filter val="一抹煙雨落繁華"/>
-        <filter val="一直梨花压海棠"/>
-        <filter val="丶天蓝色"/>
-        <filter val="丶忍野咩咩"/>
-        <filter val="伊贰叁"/>
-        <filter val="倾舞情儿"/>
-        <filter val="其实想玩刀客"/>
-        <filter val="再见是否红着脸"/>
-        <filter val="冷清语"/>
-        <filter val="凯贼阔里"/>
-        <filter val="南宫絮语"/>
-        <filter val="只想做个好人"/>
-        <filter val="在下唐银"/>
-        <filter val="墨河"/>
-        <filter val="墨韵轩华"/>
-        <filter val="天真无邪大胡子"/>
-        <filter val="太极至尊"/>
-        <filter val="女神菲奥娜"/>
-        <filter val="娇软の小屁股"/>
-        <filter val="小阿淮呀"/>
-        <filter val="山高丶木易"/>
-        <filter val="开封拍卖行"/>
-        <filter val="彼眸"/>
-        <filter val="怒怒怒怒火"/>
-        <filter val="慕容靉"/>
-        <filter val="折扇浪漫"/>
-        <filter val="明年今日奕十年"/>
-        <filter val="晓月梦澈"/>
-        <filter val="机智勇敢的小炮"/>
-        <filter val="梦觞丶"/>
-        <filter val="歌风路丶三狗蛋"/>
-        <filter val="水影悠兰"/>
-        <filter val="池小晚"/>
-        <filter val="池小猫"/>
-        <filter val="沐浠尘"/>
-        <filter val="洪时雪"/>
-        <filter val="浪迹小秦"/>
-        <filter val="淡若清风過丶"/>
-        <filter val="潇洒仗剑天下"/>
-        <filter val="爱哭鼻の阿木木"/>
-        <filter val="白芹"/>
-        <filter val="破穿"/>
-        <filter val="神威再见"/>
-        <filter val="空虚公子萧四无"/>
-        <filter val="等风与你"/>
-        <filter val="素蝶"/>
-        <filter val="紫舞流年"/>
-        <filter val="胡大力"/>
-        <filter val="艾莉亞史塔克"/>
-        <filter val="花谢人凋零。"/>
-        <filter val="超人不会飞〃"/>
-        <filter val="轻素剪云端"/>
-        <filter val="陌路莫回"/>
-        <filter val="零拾"/>
-        <filter val="青丝枫凌"/>
-        <filter val="风语风＊"/>
-        <filter val="鱼香"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:C572"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>